<commit_message>
Funciones Ver, Editar, Crear y Borrar añadidad a Proyectos
</commit_message>
<xml_diff>
--- a/Diario.xlsx
+++ b/Diario.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xlopez\Desktop\E2\E2_IW_G6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\OneDrive - Universidad de Deusto\Escritorio\E2_IW_G6\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB76F77F-E5A8-428D-8B2B-7CE955394D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Título de tarea y breve descripción </t>
   </si>
@@ -48,12 +49,18 @@
   </si>
   <si>
     <t>Crear los archivos template: base, cliente, landing y proyecto</t>
+  </si>
+  <si>
+    <t>Implementación de vistas CRUD para modelo Proyecto: Creadas las vistas genéricas para visualizar, crear, editar y eliminar proyectos. También definida la plantilla base proyecto_form.html y configurada la navegación básica entre páginas.</t>
+  </si>
+  <si>
+    <t>Unai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,23 +230,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -250,30 +279,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -558,302 +563,270 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:E14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="1" t="s">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+    <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="8" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-    </row>
-    <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-    </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="8" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="20">
+      <c r="G5" s="15"/>
+      <c r="H5" s="18">
         <v>45777</v>
       </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="16"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="16"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="16"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="15"/>
-      <c r="I19" s="15"/>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="16"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="16"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="18">
+        <v>45776</v>
+      </c>
+      <c r="I7" s="18">
+        <v>45777</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="11"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="46">
@@ -863,14 +836,14 @@
     <mergeCell ref="F23:G24"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="I23:I24"/>
+    <mergeCell ref="B21:E22"/>
+    <mergeCell ref="F21:G22"/>
     <mergeCell ref="H5:H6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="B7:E8"/>
     <mergeCell ref="F7:G8"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B21:E22"/>
-    <mergeCell ref="F21:G22"/>
     <mergeCell ref="B5:E6"/>
     <mergeCell ref="F5:G6"/>
     <mergeCell ref="B17:E18"/>

</xml_diff>

<commit_message>
Funciones añadidas a Empleado
</commit_message>
<xml_diff>
--- a/Diario.xlsx
+++ b/Diario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deusto\OneDrive - Universidad de Deusto\Escritorio\E2_IW_G6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB76F77F-E5A8-428D-8B2B-7CE955394D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4857FC93-EE59-43CA-987F-48AA6E57772A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t xml:space="preserve">Título de tarea y breve descripción </t>
   </si>
@@ -51,19 +51,30 @@
     <t>Crear los archivos template: base, cliente, landing y proyecto</t>
   </si>
   <si>
-    <t>Implementación de vistas CRUD para modelo Proyecto: Creadas las vistas genéricas para visualizar, crear, editar y eliminar proyectos. También definida la plantilla base proyecto_form.html y configurada la navegación básica entre páginas.</t>
-  </si>
-  <si>
     <t>Unai</t>
+  </si>
+  <si>
+    <t>Implementar las funciones de Proyecto: Creadas las vistas para visualizar, crear, editar y eliminar proyectos. También definida la plantilla base proyecto_form.html y configurada la navegación entre páginas.</t>
+  </si>
+  <si>
+    <t>Implementar las funciones de Empleado: Creadas las vistas para visualizar, crear, editar y eliminar empleados. También definida la plantilla base empleados_form.html y configurada la navegación entre páginas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -230,26 +241,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -282,6 +280,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -564,272 +580,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I24"/>
+  <dimension ref="B2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="18"/>
+      <c r="H2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="19" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="14" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="14" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="18">
+      <c r="G5" s="10"/>
+      <c r="H5" s="13">
         <v>45777</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="18">
+      <c r="G7" s="10"/>
+      <c r="H7" s="13">
         <v>45776</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="13">
         <v>45777</v>
       </c>
     </row>
     <row r="8" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="13">
+        <v>45778</v>
+      </c>
+      <c r="I9" s="13">
+        <v>45778</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="46">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="F3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B9:E10"/>
+    <mergeCell ref="F9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="B13:E14"/>
+    <mergeCell ref="F13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="B15:E16"/>
+    <mergeCell ref="F15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="B17:E18"/>
+    <mergeCell ref="F17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="B19:E20"/>
+    <mergeCell ref="F19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B7:E8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="F5:G6"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="B23:E24"/>
@@ -838,44 +909,6 @@
     <mergeCell ref="I23:I24"/>
     <mergeCell ref="B21:E22"/>
     <mergeCell ref="F21:G22"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B7:E8"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="B5:E6"/>
-    <mergeCell ref="F5:G6"/>
-    <mergeCell ref="B17:E18"/>
-    <mergeCell ref="F17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="B19:E20"/>
-    <mergeCell ref="F19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="B13:E14"/>
-    <mergeCell ref="F13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="B15:E16"/>
-    <mergeCell ref="F15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="B9:E10"/>
-    <mergeCell ref="F9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="B11:E12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="B3:E4"/>
-    <mergeCell ref="F3:G4"/>
-    <mergeCell ref="H3:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>